<commit_message>
Changed: updated tracker, planned next steps
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\TrainingPlanApp.Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E747E50-C46A-4CAE-B292-FB5D16DDE59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB7F440-05D0-4830-862C-50FC6098DC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Other" sheetId="1" r:id="rId1"/>
     <sheet name="Exercises" sheetId="10" r:id="rId2"/>
     <sheet name="Training Plans" sheetId="9" r:id="rId3"/>
     <sheet name="Ingredients" sheetId="8" r:id="rId4"/>
+    <sheet name="Meals" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="91">
   <si>
     <t>Pass</t>
   </si>
@@ -262,6 +263,45 @@
   </si>
   <si>
     <t>Fix string types to int types in DB and VM classes</t>
+  </si>
+  <si>
+    <t>Create meals database table - int Id, string Name, List&lt;Ingredients&gt; Ingredients</t>
+  </si>
+  <si>
+    <t>Craete MealsVM - int Id, string Name, int Kcal, int Proteins, int Carbohydrates, int Fats</t>
+  </si>
+  <si>
+    <t>IndexVM</t>
+  </si>
+  <si>
+    <t>Create meal edit view page</t>
+  </si>
+  <si>
+    <t>Create meal create view page</t>
+  </si>
+  <si>
+    <t>Create meals index view page</t>
+  </si>
+  <si>
+    <t>EditVM</t>
+  </si>
+  <si>
+    <t>Create MealsEditVM - int Id, string Name, List&lt;Ingredients&gt; Ingredients</t>
+  </si>
+  <si>
+    <t>CreateVM</t>
+  </si>
+  <si>
+    <t>Create MealsCreateVM - int Id, string Name, List&lt;Ingredients&gt; Ingredients</t>
+  </si>
+  <si>
+    <t>DetailsVM</t>
+  </si>
+  <si>
+    <t>Create MealsDetailsVM - int Id, string Name, List&lt;Ingredients&gt; Ingredients, int Kcal, int Proteins, int Carbohydrates, int Fats</t>
+  </si>
+  <si>
+    <t>Create meal details view page</t>
   </si>
 </sst>
 </file>
@@ -373,9 +413,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -389,11 +426,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -886,12 +976,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -908,7 +998,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -917,12 +1007,12 @@
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -931,12 +1021,12 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -945,12 +1035,12 @@
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -959,12 +1049,12 @@
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -973,12 +1063,12 @@
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -987,12 +1077,12 @@
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1001,12 +1091,12 @@
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1015,12 +1105,12 @@
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1029,12 +1119,12 @@
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1043,171 +1133,171 @@
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="6"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="6"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="6"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="6"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="6"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="6"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="6"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="6"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="6"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="6"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="6"/>
+      <c r="D39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1215,19 +1305,19 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C3:C39">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1259,12 +1349,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1281,7 +1371,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1290,12 +1380,12 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1304,12 +1394,12 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1318,12 +1408,12 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1332,12 +1422,12 @@
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1346,12 +1436,12 @@
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1360,12 +1450,12 @@
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1374,177 +1464,177 @@
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="6"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="6"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="6"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="6"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="6"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="6"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="6"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="6"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="6"/>
+      <c r="D37" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1552,6 +1642,421 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C3:C37">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:D37" xr:uid="{8C4AC899-F85F-4C30-AAF0-1990FA7DA92A}">
+      <formula1>"Pass, Fail, In Progress, Pending, Blocked"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF830DC-3433-4600-98E0-1D189C762893}">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="212" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="C3:C38">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
@@ -1569,7 +2074,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:D37" xr:uid="{8C4AC899-F85F-4C30-AAF0-1990FA7DA92A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C38" xr:uid="{EDBB6C6C-38A5-4E8C-9B27-67BD2D7F9C82}">
       <formula1>"Pass, Fail, In Progress, Pending, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1577,31 +2082,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF830DC-3433-4600-98E0-1D189C762893}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446ADFD5-7161-4A01-83C4-636E3045A790}">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="212" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="219.140625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1621,345 +2126,265 @@
       <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>27</v>
+      <c r="B3" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>33</v>
+        <v>76</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="D8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A13" s="7"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A14" s="7"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A15" s="7"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A16" s="7"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A17" s="7"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A18" s="7"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="5"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="5"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="5"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="5"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="5"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="5"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="5"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="5"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="5"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="5"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="5"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="2"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
-      <c r="B30" s="5"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="5"/>
+      <c r="B32" s="2"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="5"/>
+      <c r="D38" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1984,7 +2409,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C38" xr:uid="{EDBB6C6C-38A5-4E8C-9B27-67BD2D7F9C82}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C38" xr:uid="{9179387F-E73D-444B-BBBA-43095F0B9114}">
       <formula1>"Pass, Fail, In Progress, Pending, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1992,12 +2417,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446ADFD5-7161-4A01-83C4-636E3045A790}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF7D665-6E85-4367-89D8-1F66DF206E0A}">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,12 +2436,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2033,261 +2458,253 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>54</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>56</v>
+      <c r="A4" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>54</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>54</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -2296,7 +2713,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C3:C38">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Blocked"</formula>
@@ -2315,7 +2731,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C38" xr:uid="{9179387F-E73D-444B-BBBA-43095F0B9114}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C38" xr:uid="{8F45D321-8C0E-48B8-9314-D141F9963A75}">
       <formula1>"Pass, Fail, In Progress, Pending, Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changed: Meal table, MealVM; Added: method counting the macros of the meals in database
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\TrainingPlanApp.Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB7F440-05D0-4830-862C-50FC6098DC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E41034-FD9D-40CD-AB16-BC1296A49939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Training Plans" sheetId="9" r:id="rId3"/>
     <sheet name="Ingredients" sheetId="8" r:id="rId4"/>
     <sheet name="Meals" sheetId="12" r:id="rId5"/>
+    <sheet name="Arkusz1" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -265,9 +266,6 @@
     <t>Fix string types to int types in DB and VM classes</t>
   </si>
   <si>
-    <t>Create meals database table - int Id, string Name, List&lt;Ingredients&gt; Ingredients</t>
-  </si>
-  <si>
     <t>Craete MealsVM - int Id, string Name, int Kcal, int Proteins, int Carbohydrates, int Fats</t>
   </si>
   <si>
@@ -302,6 +300,9 @@
   </si>
   <si>
     <t>Create meal details view page</t>
+  </si>
+  <si>
+    <t>Create meals database table - int Id, string Name, List&lt;int&gt; IngredientId, string Recipe</t>
   </si>
 </sst>
 </file>
@@ -2422,7 +2423,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,17 +2463,17 @@
         <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="5"/>
@@ -2482,17 +2483,17 @@
         <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="5"/>
@@ -2502,17 +2503,17 @@
         <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="5"/>
@@ -2522,17 +2523,17 @@
         <v>60</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="5"/>
@@ -2542,7 +2543,7 @@
         <v>62</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="5"/>
@@ -2737,4 +2738,16 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166665FC-1C4F-4067-9060-5E17D63013E9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added: macros view to manageingredientsview - code polishing required
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\TrainingPlanApp.Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E41034-FD9D-40CD-AB16-BC1296A49939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961FBF12-1C7A-47F9-9A7C-5093B417A90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="95">
   <si>
     <t>Pass</t>
   </si>
@@ -303,6 +303,18 @@
   </si>
   <si>
     <t>Create meals database table - int Id, string Name, List&lt;int&gt; IngredientId, string Recipe</t>
+  </si>
+  <si>
+    <t>GetMacrosOfTheMeals</t>
+  </si>
+  <si>
+    <t>Method that counts up kcal, proteins, fats, and carbs of all meals in the database</t>
+  </si>
+  <si>
+    <t>GetMacroOfTheMeal</t>
+  </si>
+  <si>
+    <t>Method that counts up kcal, proteins, fats, and carbs of single meal</t>
   </si>
 </sst>
 </file>
@@ -2423,7 +2435,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,8 +2477,12 @@
       <c r="B3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -2475,7 +2491,9 @@
       <c r="B4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2485,7 +2503,9 @@
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2495,7 +2515,9 @@
       <c r="B6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2561,14 +2583,26 @@
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="5"/>
     </row>

</xml_diff>